<commit_message>
update register account info
</commit_message>
<xml_diff>
--- a/src/test/java/nopcommerce4/LT2/utilities/ExcelData.xlsx
+++ b/src/test/java/nopcommerce4/LT2/utilities/ExcelData.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17160" windowHeight="2544" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17160" windowHeight="2136" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:N5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,10 +65,10 @@
     <t>testschool</t>
   </si>
   <si>
-    <t>testLT005</t>
-  </si>
-  <si>
-    <t>testLT005@test.com</t>
+    <t>testLT006</t>
+  </si>
+  <si>
+    <t>testLT006@test.com</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>